<commit_message>
add tests to validate processing of DNSSEC parameters
</commit_message>
<xml_diff>
--- a/data/epp-14-data.xlsx
+++ b/data/epp-14-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/icann/rst-test-specs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7A2833-C1CE-5645-89AE-666A6B382C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771F4ED2-EAD7-5F4E-98DE-33825E5AC6A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="2340" windowWidth="35460" windowHeight="17220" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
+    <workbookView xWindow="1020" yWindow="2340" windowWidth="35460" windowHeight="17220" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="99">
   <si>
     <t>errorCode</t>
   </si>
@@ -298,6 +298,93 @@
   </si>
   <si>
     <t>attributes</t>
+  </si>
+  <si>
+    <t>keyTag</t>
+  </si>
+  <si>
+    <t>digestType</t>
+  </si>
+  <si>
+    <t>digest</t>
+  </si>
+  <si>
+    <t>flags</t>
+  </si>
+  <si>
+    <t>protocol</t>
+  </si>
+  <si>
+    <t>pubKey</t>
+  </si>
+  <si>
+    <t>keyDataAlg</t>
+  </si>
+  <si>
+    <t>dsDataAlg</t>
+  </si>
+  <si>
+    <t>DS record Key Tag (if applicable)</t>
+  </si>
+  <si>
+    <t>DS record algorithm (if applicable)</t>
+  </si>
+  <si>
+    <t>DS record digest type (if applicable)</t>
+  </si>
+  <si>
+    <t>DS record digest (if applicable)</t>
+  </si>
+  <si>
+    <t>DNSKEY record flags (if applicable)</t>
+  </si>
+  <si>
+    <t>DNSKEY record protocol (if applicable)</t>
+  </si>
+  <si>
+    <t>DNSKEY record algorithm (if applicable)</t>
+  </si>
+  <si>
+    <t>DNSKEY record public key (if applicable)</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>{RANDHEX(32}</t>
+  </si>
+  <si>
+    <t>257</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>7JCMl8WwNOyFNWF6GBuMlIdtf08Cr1bO/hToZ6xCvKcu4o5ShXBzbCgzTGJHovhoUgj9wsMA1aWA</t>
+  </si>
+  <si>
+    <t>EPP_DOMAIN_CREATE_SERVER_ACCEPTS_INVALID_DNSSEC_DATA</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>255</t>
+  </si>
+  <si>
+    <t>{RANDHEX(32})</t>
+  </si>
+  <si>
+    <t>256</t>
+  </si>
+  <si>
+    <t>this is not a DNSKEY.</t>
   </si>
 </sst>
 </file>
@@ -414,7 +501,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="26">
     <dxf>
       <font>
         <b val="0"/>
@@ -437,26 +524,186 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -769,8 +1016,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:Q33" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="B7:Q33" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:Y59" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="B7:Y59" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -787,24 +1034,40 @@
     <filterColumn colId="13" hiddenButton="1"/>
     <filterColumn colId="14" hiddenButton="1"/>
     <filterColumn colId="15" hiddenButton="1"/>
+    <filterColumn colId="16" hiddenButton="1"/>
+    <filterColumn colId="17" hiddenButton="1"/>
+    <filterColumn colId="18" hiddenButton="1"/>
+    <filterColumn colId="19" hiddenButton="1"/>
+    <filterColumn colId="20" hiddenButton="1"/>
+    <filterColumn colId="21" hiddenButton="1"/>
+    <filterColumn colId="22" hiddenButton="1"/>
+    <filterColumn colId="23" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{4AE738EA-0F6E-7D4F-8E30-1F60F72D5773}" name="name" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{9D2F85A4-8ECB-0C46-BF52-02059D67DF93}" name="period" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{F674F9C4-5917-5641-A4A5-837679F19176}" name="periodUnit" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{34E04925-4A89-B94E-872A-054A44B06DAB}" name="registrant" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{2D040C66-74F7-FA40-8F80-4EFBCBB7D804}" name="adminContact" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{0171B6E3-C679-0646-B61B-94DDF6D0739F}" name="techContact" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{C8B4F55C-77A5-2B43-B03E-20E1A6AC72EC}" name="billingContact" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{E760EB62-F451-2C49-A376-7B991B84B914}" name="hostModel" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{D5A9FB71-E997-F340-BA79-F64CC55AECE4}" name="ns1" dataDxfId="8"/>
-    <tableColumn id="12" xr3:uid="{8EE92E73-77B7-A542-82BA-CB74FCA1CB5A}" name="ns1ipv4" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{C1C56F35-E74B-2140-B92B-289F873FF934}" name="ns1ipv6" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{8F31D634-EEAA-0141-B19B-197F1349C252}" name="ns2" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{001B761F-29C1-EE41-99B2-E2116E52D500}" name="ns2ipv4" dataDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{FF7943E7-C72F-BB41-8084-CBEE83A6C9D2}" name="ns2ipv6" dataDxfId="3"/>
-    <tableColumn id="15" xr3:uid="{00D82E93-146D-6544-AF62-0DE540BD8AA2}" name="passOrFail" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{8BB18A73-00AF-4640-8340-D626F25C4C5F}" name="errorCode" dataDxfId="1"/>
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{4AE738EA-0F6E-7D4F-8E30-1F60F72D5773}" name="name" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{9D2F85A4-8ECB-0C46-BF52-02059D67DF93}" name="period" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{F674F9C4-5917-5641-A4A5-837679F19176}" name="periodUnit" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{34E04925-4A89-B94E-872A-054A44B06DAB}" name="registrant" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{2D040C66-74F7-FA40-8F80-4EFBCBB7D804}" name="adminContact" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{0171B6E3-C679-0646-B61B-94DDF6D0739F}" name="techContact" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{C8B4F55C-77A5-2B43-B03E-20E1A6AC72EC}" name="billingContact" dataDxfId="17"/>
+    <tableColumn id="17" xr3:uid="{E760EB62-F451-2C49-A376-7B991B84B914}" name="hostModel" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{D5A9FB71-E997-F340-BA79-F64CC55AECE4}" name="ns1" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{8EE92E73-77B7-A542-82BA-CB74FCA1CB5A}" name="ns1ipv4" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{C1C56F35-E74B-2140-B92B-289F873FF934}" name="ns1ipv6" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{8F31D634-EEAA-0141-B19B-197F1349C252}" name="ns2" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{001B761F-29C1-EE41-99B2-E2116E52D500}" name="ns2ipv4" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{FF7943E7-C72F-BB41-8084-CBEE83A6C9D2}" name="ns2ipv6" dataDxfId="10"/>
+    <tableColumn id="20" xr3:uid="{84610D9D-62D8-C747-BEB0-DA340D34D421}" name="keyTag" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{54D27880-56AD-DC42-BE78-EBB1A19D2339}" name="dsDataAlg" dataDxfId="5"/>
+    <tableColumn id="18" xr3:uid="{4C2A616C-31AB-9948-877D-701A0692DECD}" name="digestType" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{2467371F-CDC1-0443-9301-00252404EE8B}" name="digest" dataDxfId="7"/>
+    <tableColumn id="24" xr3:uid="{66E3B520-5E7B-914A-A7E7-5D2A0EC1B025}" name="flags" dataDxfId="0"/>
+    <tableColumn id="23" xr3:uid="{85CBAD45-FEDA-EF41-B68C-A469EEC82B26}" name="protocol" dataDxfId="1"/>
+    <tableColumn id="22" xr3:uid="{7BF4016C-657D-B647-BB2B-87573194BAB3}" name="keyDataAlg" dataDxfId="2"/>
+    <tableColumn id="21" xr3:uid="{D26FFFA2-9A10-9943-A61D-4B69D6D32E34}" name="pubKey" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{00D82E93-146D-6544-AF62-0DE540BD8AA2}" name="passOrFail" dataDxfId="9"/>
+    <tableColumn id="16" xr3:uid="{8BB18A73-00AF-4640-8340-D626F25C4C5F}" name="errorCode" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1127,10 +1390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D4FAA1-1060-DC4E-8B86-313DD9301EC2}">
-  <dimension ref="B2:X33"/>
+  <dimension ref="B2:AF59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="M5" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1147,12 +1410,14 @@
     <col min="11" max="12" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="88.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="1"/>
+    <col min="16" max="22" width="16" style="1" customWidth="1"/>
+    <col min="23" max="23" width="95" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="88.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" ht="25" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:32" ht="25" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
@@ -1171,8 +1436,16 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
-    </row>
-    <row r="3" spans="2:24" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+    </row>
+    <row r="3" spans="2:32" ht="114" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
         <v>41</v>
       </c>
@@ -1198,8 +1471,16 @@
       <c r="V3" s="10"/>
       <c r="W3" s="10"/>
       <c r="X3" s="10"/>
-    </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+      <c r="AC3" s="10"/>
+      <c r="AD3" s="10"/>
+      <c r="AE3" s="10"/>
+      <c r="AF3" s="10"/>
+    </row>
+    <row r="4" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -1216,8 +1497,16 @@
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
-    </row>
-    <row r="5" spans="2:24" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+    </row>
+    <row r="5" spans="2:32" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
@@ -1236,8 +1525,16 @@
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
-    </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+    </row>
+    <row r="6" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -1254,8 +1551,16 @@
       <c r="O6" s="8"/>
       <c r="P6" s="8"/>
       <c r="Q6" s="8"/>
-    </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+    </row>
+    <row r="7" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1299,13 +1604,37 @@
         <v>48</v>
       </c>
       <c r="P7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="X7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Y7" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:24" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:32" s="3" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
@@ -1349,13 +1678,37 @@
         <v>45</v>
       </c>
       <c r="P8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="X8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="Y8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
@@ -1399,13 +1752,37 @@
         <v>3</v>
       </c>
       <c r="P9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Q9" s="4" t="s">
+      <c r="T9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="W9" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="X9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y9" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1449,110 +1826,134 @@
         <v>46</v>
       </c>
       <c r="P10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="X10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Y10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="P11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="1" t="s">
+      <c r="X11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="1" t="s">
+      <c r="X12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="X13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="Y13" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:32" x14ac:dyDescent="0.2">
       <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="1" t="s">
+      <c r="X14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:32" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="1" t="s">
+      <c r="X15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:32" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="1" t="s">
+      <c r="X16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="P17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="1" t="s">
+      <c r="X17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:25" x14ac:dyDescent="0.2">
       <c r="D18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="P18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="1" t="s">
+      <c r="X18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:25" x14ac:dyDescent="0.2">
       <c r="E19" s="1" t="s">
         <v>14</v>
       </c>
@@ -1562,28 +1963,28 @@
       <c r="G19" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="1" t="s">
+      <c r="X19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:25" x14ac:dyDescent="0.2">
       <c r="G20" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P20" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="1" t="s">
+      <c r="X20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:25" x14ac:dyDescent="0.2">
       <c r="H21" s="1" t="s">
         <v>40</v>
       </c>
@@ -1593,155 +1994,465 @@
       <c r="J21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="P21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="1" t="s">
+      <c r="X21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:25" x14ac:dyDescent="0.2">
       <c r="K22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="X22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="Y22" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:25" x14ac:dyDescent="0.2">
       <c r="K23" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="P23" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q23" s="1" t="s">
+      <c r="X23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:25" x14ac:dyDescent="0.2">
       <c r="K24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="P24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q24" s="1" t="s">
+      <c r="X24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:25" x14ac:dyDescent="0.2">
       <c r="K25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="P25" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="1" t="s">
+      <c r="X25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:25" x14ac:dyDescent="0.2">
       <c r="K26" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="P26" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="1" t="s">
+      <c r="X26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:25" x14ac:dyDescent="0.2">
       <c r="K27" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="P27" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q27" s="1" t="s">
+      <c r="X27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:25" x14ac:dyDescent="0.2">
       <c r="K28" s="1" t="s">
         <v>46</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="P28" s="1" t="s">
+      <c r="X28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q28" s="1" t="s">
+      <c r="Y28" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:25" x14ac:dyDescent="0.2">
       <c r="L29" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="P29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q29" s="1" t="s">
+      <c r="X29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y29" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:25" x14ac:dyDescent="0.2">
       <c r="L30" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="P30" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q30" s="1" t="s">
+      <c r="X30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y30" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:25" x14ac:dyDescent="0.2">
       <c r="L31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="P31" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q31" s="1" t="s">
+      <c r="X31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y31" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="3:17" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:25" x14ac:dyDescent="0.2">
       <c r="L32" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="P32" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q32" s="1" t="s">
+      <c r="X32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y32" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="12:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="10:25" x14ac:dyDescent="0.2">
       <c r="L33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="P33" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q33" s="1" t="s">
+      <c r="X33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y33" s="1" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="10:25" x14ac:dyDescent="0.2">
+      <c r="J34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X34" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y34" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="10:25" x14ac:dyDescent="0.2">
+      <c r="P35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y35" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="10:25" x14ac:dyDescent="0.2">
+      <c r="Q36" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y36" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="10:25" x14ac:dyDescent="0.2">
+      <c r="Q37" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="X37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y37" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="10:25" x14ac:dyDescent="0.2">
+      <c r="Q38" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y38" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="39" spans="10:25" x14ac:dyDescent="0.2">
+      <c r="Q39" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y39" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="40" spans="10:25" x14ac:dyDescent="0.2">
+      <c r="R40" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y40" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="10:25" x14ac:dyDescent="0.2">
+      <c r="R41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="X41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y41" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="10:25" x14ac:dyDescent="0.2">
+      <c r="R42" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="X42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y42" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="43" spans="10:25" x14ac:dyDescent="0.2">
+      <c r="R43" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="S43" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y43" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="10:25" x14ac:dyDescent="0.2">
+      <c r="S44" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="T44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y44" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="10:25" x14ac:dyDescent="0.2">
+      <c r="T45" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y45" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="10:25" x14ac:dyDescent="0.2">
+      <c r="T46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="X46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y46" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="10:25" x14ac:dyDescent="0.2">
+      <c r="T47" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y47" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="10:25" x14ac:dyDescent="0.2">
+      <c r="T48" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="X48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y48" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="20:25" x14ac:dyDescent="0.2">
+      <c r="T49" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="U49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y49" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="20:25" x14ac:dyDescent="0.2">
+      <c r="U50" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="X50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y50" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="20:25" x14ac:dyDescent="0.2">
+      <c r="U51" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="X51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y51" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="20:25" x14ac:dyDescent="0.2">
+      <c r="U52" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y52" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="20:25" x14ac:dyDescent="0.2">
+      <c r="U53" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="X53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y53" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="20:25" x14ac:dyDescent="0.2">
+      <c r="U54" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="V54" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y54" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="20:25" x14ac:dyDescent="0.2">
+      <c r="V55" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y55" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="20:25" x14ac:dyDescent="0.2">
+      <c r="V56" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="X56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y56" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="20:25" x14ac:dyDescent="0.2">
+      <c r="V57" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="X57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y57" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="20:25" x14ac:dyDescent="0.2">
+      <c r="V58" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="W58" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="X58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y58" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="59" spans="20:25" x14ac:dyDescent="0.2">
+      <c r="W59" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="X59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y59" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="B5:Q5"/>
-    <mergeCell ref="B4:Q4"/>
-    <mergeCell ref="B6:Q6"/>
-    <mergeCell ref="B3:X3"/>
+    <mergeCell ref="B2:Y2"/>
+    <mergeCell ref="B5:Y5"/>
+    <mergeCell ref="B4:Y4"/>
+    <mergeCell ref="B6:Y6"/>
+    <mergeCell ref="B3:AF3"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add secDNSInterface column (closes #50)
</commit_message>
<xml_diff>
--- a/data/epp-14-data.xlsx
+++ b/data/epp-14-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gavin.brown/Code/rst-test-specs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045ACB67-2F81-744F-9E0D-2A59CDAFBE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5048BE27-AAC6-694A-BBD9-0720B2C6D77D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{CD472396-4CFB-9A45-AA99-46F4E9CB8B91}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="103">
   <si>
     <t>errorCode</t>
   </si>
@@ -350,6 +350,18 @@
 * Empty cells do not indicate an empty string (the "{EMPTY}" value indicates that), but will be replaced with the value in the previous row when this file is converted into YAML.
 * This means that all cells in the first row MUST be populated.
 * IP addresses must be taken from the prefixes 208.77.190.192/26 and 2602:800:900e:1257::/64 and should not be reused.</t>
+  </si>
+  <si>
+    <t>secDNSInterface</t>
+  </si>
+  <si>
+    <t>Data interface (see RFC 5910, row will be skipped if the value does not match the epp.secDNSInterfaces input parameter)</t>
+  </si>
+  <si>
+    <t>dsData</t>
+  </si>
+  <si>
+    <t>keyData</t>
   </si>
 </sst>
 </file>
@@ -479,7 +491,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="25">
     <dxf>
       <font>
         <strike val="0"/>
@@ -502,6 +514,26 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
         <color theme="1"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -954,8 +986,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:W59" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="B7:W59" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}" name="DataProvider" displayName="DataProvider" ref="B7:X59" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="B7:X59" xr:uid="{E85A8946-EC69-EC4F-9D2F-ABC371B76D30}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -978,20 +1010,22 @@
     <filterColumn colId="19" hiddenButton="1"/>
     <filterColumn colId="20" hiddenButton="1"/>
     <filterColumn colId="21" hiddenButton="1"/>
+    <filterColumn colId="22" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="22">
-    <tableColumn id="1" xr3:uid="{4AE738EA-0F6E-7D4F-8E30-1F60F72D5773}" name="name" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{9D2F85A4-8ECB-0C46-BF52-02059D67DF93}" name="period" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{F674F9C4-5917-5641-A4A5-837679F19176}" name="periodUnit" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{290FD370-EDF0-6446-9EB7-23A938BC4FA1}" name="dataModel" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{34E04925-4A89-B94E-872A-054A44B06DAB}" name="registrant" dataDxfId="17"/>
-    <tableColumn id="17" xr3:uid="{E760EB62-F451-2C49-A376-7B991B84B914}" name="hostModel" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{D5A9FB71-E997-F340-BA79-F64CC55AECE4}" name="ns1" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{8EE92E73-77B7-A542-82BA-CB74FCA1CB5A}" name="ns1ipv4" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{C1C56F35-E74B-2140-B92B-289F873FF934}" name="ns1ipv6" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{8F31D634-EEAA-0141-B19B-197F1349C252}" name="ns2" dataDxfId="12"/>
-    <tableColumn id="13" xr3:uid="{001B761F-29C1-EE41-99B2-E2116E52D500}" name="ns2ipv4" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{FF7943E7-C72F-BB41-8084-CBEE83A6C9D2}" name="ns2ipv6" dataDxfId="10"/>
+  <tableColumns count="23">
+    <tableColumn id="1" xr3:uid="{4AE738EA-0F6E-7D4F-8E30-1F60F72D5773}" name="name" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{9D2F85A4-8ECB-0C46-BF52-02059D67DF93}" name="period" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{F674F9C4-5917-5641-A4A5-837679F19176}" name="periodUnit" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{290FD370-EDF0-6446-9EB7-23A938BC4FA1}" name="dataModel" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{34E04925-4A89-B94E-872A-054A44B06DAB}" name="registrant" dataDxfId="18"/>
+    <tableColumn id="17" xr3:uid="{E760EB62-F451-2C49-A376-7B991B84B914}" name="hostModel" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{D5A9FB71-E997-F340-BA79-F64CC55AECE4}" name="ns1" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{8EE92E73-77B7-A542-82BA-CB74FCA1CB5A}" name="ns1ipv4" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{C1C56F35-E74B-2140-B92B-289F873FF934}" name="ns1ipv6" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{8F31D634-EEAA-0141-B19B-197F1349C252}" name="ns2" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{001B761F-29C1-EE41-99B2-E2116E52D500}" name="ns2ipv4" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{FF7943E7-C72F-BB41-8084-CBEE83A6C9D2}" name="ns2ipv6" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{D990300C-9C03-814D-B2C0-A5B615F7F5B0}" name="secDNSInterface" dataDxfId="10"/>
     <tableColumn id="20" xr3:uid="{84610D9D-62D8-C747-BEB0-DA340D34D421}" name="keyTag" dataDxfId="9"/>
     <tableColumn id="19" xr3:uid="{54D27880-56AD-DC42-BE78-EBB1A19D2339}" name="dsDataAlg" dataDxfId="8"/>
     <tableColumn id="18" xr3:uid="{4C2A616C-31AB-9948-877D-701A0692DECD}" name="digestType" dataDxfId="7"/>
@@ -1324,10 +1358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21D4FAA1-1060-DC4E-8B86-313DD9301EC2}">
-  <dimension ref="B2:AD59"/>
+  <dimension ref="B2:AE59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:W5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1343,20 +1377,21 @@
     <col min="10" max="10" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="95" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="88.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="10.83203125" style="1"/>
+    <col min="14" max="14" width="17.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="95" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="88.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:30" ht="25" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:31" ht="25" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
@@ -1381,8 +1416,9 @@
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
-    </row>
-    <row r="3" spans="2:30" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="X2" s="6"/>
+    </row>
+    <row r="3" spans="2:31" ht="114" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
         <v>91</v>
       </c>
@@ -1414,8 +1450,9 @@
       <c r="AB3" s="11"/>
       <c r="AC3" s="11"/>
       <c r="AD3" s="11"/>
-    </row>
-    <row r="4" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AE3" s="11"/>
+    </row>
+    <row r="4" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
@@ -1438,8 +1475,9 @@
       <c r="U4" s="8"/>
       <c r="V4" s="8"/>
       <c r="W4" s="8"/>
-    </row>
-    <row r="5" spans="2:30" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="X4" s="8"/>
+    </row>
+    <row r="5" spans="2:31" ht="128" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>98</v>
       </c>
@@ -1464,8 +1502,9 @@
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
       <c r="W5" s="7"/>
-    </row>
-    <row r="6" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="X5" s="7"/>
+    </row>
+    <row r="6" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -1488,8 +1527,9 @@
       <c r="U6" s="9"/>
       <c r="V6" s="9"/>
       <c r="W6" s="9"/>
-    </row>
-    <row r="7" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="X6" s="9"/>
+    </row>
+    <row r="7" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
@@ -1527,37 +1567,40 @@
         <v>36</v>
       </c>
       <c r="N7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="O7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="P7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="T7" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="U7" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="V7" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="W7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:30" s="3" customFormat="1" ht="91" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:31" s="3" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
         <v>16</v>
@@ -1593,37 +1636,40 @@
         <v>33</v>
       </c>
       <c r="N8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="O8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="Q8" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="Q8" s="2" t="s">
+      <c r="R8" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="S8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="S8" s="2" t="s">
+      <c r="T8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="T8" s="2" t="s">
+      <c r="U8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="U8" s="2" t="s">
+      <c r="V8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="V8" s="2" t="s">
+      <c r="W8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="W8" s="2" t="s">
+      <c r="X8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
@@ -1661,7 +1707,7 @@
         <v>3</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="O9" s="4" t="s">
         <v>17</v>
@@ -1670,10 +1716,10 @@
         <v>17</v>
       </c>
       <c r="Q9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R9" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="R9" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="S9" s="4" t="s">
         <v>17</v>
@@ -1682,7 +1728,7 @@
         <v>17</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="V9" s="4" t="s">
         <v>3</v>
@@ -1690,8 +1736,11 @@
       <c r="W9" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="X9" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>88</v>
       </c>
@@ -1729,131 +1778,134 @@
         <v>34</v>
       </c>
       <c r="N10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="S10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="T10" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="U10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="V10" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="V11" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X11" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="V12" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X12" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="V13" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:31" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>88</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="V14" s="1" t="s">
+      <c r="W14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="W14" s="1" t="s">
+      <c r="X14" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:31" x14ac:dyDescent="0.2">
       <c r="C15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="V15" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X15" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:31" x14ac:dyDescent="0.2">
       <c r="C16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V16" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X16" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="V17" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X17" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="V18" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X18" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:24" x14ac:dyDescent="0.2">
       <c r="D19" s="1" t="s">
         <v>15</v>
       </c>
@@ -1863,25 +1915,25 @@
       <c r="F19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="V19" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X19" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:24" x14ac:dyDescent="0.2">
       <c r="F20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="V20" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X20" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:24" x14ac:dyDescent="0.2">
       <c r="E21" s="1" t="s">
         <v>82</v>
       </c>
@@ -1894,465 +1946,471 @@
       <c r="H21" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="V21" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X21" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:24" x14ac:dyDescent="0.2">
       <c r="I22" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="V22" s="1" t="s">
+      <c r="W22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="W22" s="1" t="s">
+      <c r="X22" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:24" x14ac:dyDescent="0.2">
       <c r="I23" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="V23" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X23" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:24" x14ac:dyDescent="0.2">
       <c r="I24" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="V24" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:24" x14ac:dyDescent="0.2">
       <c r="I25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="V25" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X25" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:24" x14ac:dyDescent="0.2">
       <c r="I26" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="V26" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X26" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:24" x14ac:dyDescent="0.2">
       <c r="I27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="V27" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W27" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X27" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:24" x14ac:dyDescent="0.2">
       <c r="I28" s="1" t="s">
         <v>34</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="V28" s="1" t="s">
+      <c r="W28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="W28" s="1" t="s">
+      <c r="X28" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:24" x14ac:dyDescent="0.2">
       <c r="J29" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="V29" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W29" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X29" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:24" x14ac:dyDescent="0.2">
       <c r="J30" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="V30" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X30" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:24" x14ac:dyDescent="0.2">
       <c r="J31" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="V31" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X31" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="3:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:24" x14ac:dyDescent="0.2">
       <c r="J32" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="V32" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X32" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="8:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="8:24" x14ac:dyDescent="0.2">
       <c r="J33" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="V33" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X33" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="8:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="8:24" x14ac:dyDescent="0.2">
       <c r="H34" s="1" t="s">
         <v>34</v>
       </c>
       <c r="N34" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="O34" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="V34" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W34" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="N35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X34" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="8:24" x14ac:dyDescent="0.2">
+      <c r="O35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O35" s="1" t="s">
+      <c r="P35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="V35" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W35" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="O36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X35" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="8:24" x14ac:dyDescent="0.2">
+      <c r="P36" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V36" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W36" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="37" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="O37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X36" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="8:24" x14ac:dyDescent="0.2">
+      <c r="P37" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="V37" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W37" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="38" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="O38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X37" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="8:24" x14ac:dyDescent="0.2">
+      <c r="P38" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="V38" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W38" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="39" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="O39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X38" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="39" spans="8:24" x14ac:dyDescent="0.2">
+      <c r="P39" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="P39" s="1" t="s">
+      <c r="Q39" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="V39" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W39" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="40" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="P40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X39" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="40" spans="8:24" x14ac:dyDescent="0.2">
+      <c r="Q40" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V40" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W40" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="41" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="P41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X40" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="8:24" x14ac:dyDescent="0.2">
+      <c r="Q41" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="V41" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W41" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="P42" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X41" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42" spans="8:24" x14ac:dyDescent="0.2">
+      <c r="Q42" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="V42" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W42" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="43" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="P43" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X42" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="8:24" x14ac:dyDescent="0.2">
+      <c r="Q43" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="Q43" s="1" t="s">
+      <c r="R43" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="V43" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W43" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="44" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="Q44" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X43" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="8:24" x14ac:dyDescent="0.2">
+      <c r="N44" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="R44" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="R44" s="1" t="s">
+      <c r="S44" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="V44" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W44" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="R45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X44" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="8:24" x14ac:dyDescent="0.2">
+      <c r="S45" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V45" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W45" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="R46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X45" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="8:24" x14ac:dyDescent="0.2">
+      <c r="S46" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="V46" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W46" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="47" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="R47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X46" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="8:24" x14ac:dyDescent="0.2">
+      <c r="S47" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V47" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W47" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="R48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X47" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="48" spans="8:24" x14ac:dyDescent="0.2">
+      <c r="S48" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="V48" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W48" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="49" spans="18:23" x14ac:dyDescent="0.2">
-      <c r="R49" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X48" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="19:24" x14ac:dyDescent="0.2">
+      <c r="S49" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="S49" s="1" t="s">
+      <c r="T49" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="V49" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W49" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="50" spans="18:23" x14ac:dyDescent="0.2">
-      <c r="S50" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X49" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="19:24" x14ac:dyDescent="0.2">
+      <c r="T50" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V50" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W50" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="51" spans="18:23" x14ac:dyDescent="0.2">
-      <c r="S51" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X50" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="19:24" x14ac:dyDescent="0.2">
+      <c r="T51" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="V51" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W51" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="52" spans="18:23" x14ac:dyDescent="0.2">
-      <c r="S52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X51" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="19:24" x14ac:dyDescent="0.2">
+      <c r="T52" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V52" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W52" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="18:23" x14ac:dyDescent="0.2">
-      <c r="S53" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X52" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="19:24" x14ac:dyDescent="0.2">
+      <c r="T53" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="V53" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W53" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="54" spans="18:23" x14ac:dyDescent="0.2">
-      <c r="S54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X53" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="19:24" x14ac:dyDescent="0.2">
+      <c r="T54" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="T54" s="1" t="s">
+      <c r="U54" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="V54" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W54" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="55" spans="18:23" x14ac:dyDescent="0.2">
-      <c r="T55" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X54" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="19:24" x14ac:dyDescent="0.2">
+      <c r="U55" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="V55" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W55" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="56" spans="18:23" x14ac:dyDescent="0.2">
-      <c r="T56" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X55" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="19:24" x14ac:dyDescent="0.2">
+      <c r="U56" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="V56" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W56" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="57" spans="18:23" x14ac:dyDescent="0.2">
-      <c r="T57" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X56" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="19:24" x14ac:dyDescent="0.2">
+      <c r="U57" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="V57" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W57" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="58" spans="18:23" x14ac:dyDescent="0.2">
-      <c r="T58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X57" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="19:24" x14ac:dyDescent="0.2">
+      <c r="U58" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="U58" s="1" t="s">
+      <c r="V58" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="V58" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W58" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="59" spans="18:23" x14ac:dyDescent="0.2">
-      <c r="U59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X58" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="19:24" x14ac:dyDescent="0.2">
+      <c r="V59" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="V59" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="W59" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X59" s="1" t="s">
         <v>73</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B2:W2"/>
-    <mergeCell ref="B5:W5"/>
-    <mergeCell ref="B4:W4"/>
-    <mergeCell ref="B6:W6"/>
-    <mergeCell ref="B3:AD3"/>
+    <mergeCell ref="B2:X2"/>
+    <mergeCell ref="B5:X5"/>
+    <mergeCell ref="B4:X4"/>
+    <mergeCell ref="B6:X6"/>
+    <mergeCell ref="B3:AE3"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>